<commit_message>
Updated Group Test Case
</commit_message>
<xml_diff>
--- a/GroupAssignmentTestCases.xlsx
+++ b/GroupAssignmentTestCases.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -115,10 +114,6 @@
     <t>To verify that user is not being able to purchase items from order list with a balance less than total price of items</t>
   </si>
   <si>
-    <t>OS: Windows 8.1
-Browser: Chrome 41</t>
-  </si>
-  <si>
     <t>To verify that prefix validation</t>
   </si>
   <si>
@@ -252,6 +247,10 @@
   </si>
   <si>
     <t>Sumanth Yerra</t>
+  </si>
+  <si>
+    <t>OS: Windows 7
+IDE: Eclipse Luna</t>
   </si>
 </sst>
 </file>
@@ -638,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,40 +722,40 @@
         <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="L2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="M2" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,40 +769,40 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="O3" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M3" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -817,40 +816,40 @@
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="K4" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P4" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M4" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O4" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="90" x14ac:dyDescent="0.25">
@@ -864,40 +863,40 @@
         <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="O5" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P5" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M5" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O5" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -908,43 +907,43 @@
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="O6" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M6" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O6" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -958,40 +957,40 @@
         <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="O7" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P7" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M7" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O7" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1002,43 +1001,43 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O8" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P8" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M8" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O8" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="150" x14ac:dyDescent="0.25">
@@ -1049,43 +1048,43 @@
         <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="O9" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P9" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M9" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O9" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1099,40 +1098,40 @@
         <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="O10" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P10" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M10" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O10" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -1146,40 +1145,40 @@
         <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="5">
+        <v>42481</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="O11" s="5">
+        <v>42481</v>
+      </c>
+      <c r="P11" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="M11" s="5">
-        <v>42481</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O11" s="5">
-        <v>42481</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>